<commit_message>
Update to the file loop for accessing the digitized climate data, transcribing it, saving the preprocessed transcribed data and finally saving the postprocessed data in right path/folders
</commit_message>
<xml_diff>
--- a/Cross_checked_Excel_with_OCR_Results.xlsx
+++ b/Cross_checked_Excel_with_OCR_Results.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA47"/>
+  <dimension ref="A1:AB47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,53 +434,146 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Abri</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
-      <c r="H1" t="inlineStr"/>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Piche</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr"/>
-      <c r="K1" t="inlineStr"/>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>(Psychromètre a aspiration)</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr"/>
-      <c r="N1" t="inlineStr"/>
-      <c r="O1" t="inlineStr"/>
-      <c r="P1" t="inlineStr"/>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>(Psychromètre a aspiration)</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr"/>
-      <c r="S1" t="inlineStr"/>
-      <c r="T1" t="inlineStr"/>
-      <c r="U1" t="inlineStr"/>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>(Psychromètre a aspiration)</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr"/>
-      <c r="X1" t="inlineStr"/>
-      <c r="Y1" t="inlineStr"/>
-      <c r="Z1" t="inlineStr"/>
-      <c r="AA1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>No de la pentade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Bellani (gr. Cal/cm2) 6-6h</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Températures extrêmes</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Evaportation en cm3 6 - 6h</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pluies en mm. 6-6h</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Température et Humidité de l'air à 6 heures</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 12</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 13</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 14</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 15</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Température et Humidité de l'air à 15 heures</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 17</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 18</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 19</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 20</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Température et Humidité de l'air à 18 heures</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 22</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 23</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 24</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 25</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Date.1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -476,301 +581,210 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Max.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Min.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>(M+m)/2</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Ampl.</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Min. gazon</t>
-        </is>
-      </c>
+          <t>Abri</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Abri.</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Ext.</t>
-        </is>
-      </c>
+          <t>Piche</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr">
         <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>T'a</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>e.</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>∆e</t>
-        </is>
-      </c>
+          <t>(Psychromètre a aspiration)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>T'a</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>e.</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>∆e</t>
-        </is>
-      </c>
+          <t>(Psychromètre a aspiration)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr">
         <is>
-          <t>T</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>T'a</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>e.</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>U</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>∆e</t>
-        </is>
-      </c>
+          <t>(Psychromètre a aspiration)</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>825</v>
-      </c>
-      <c r="B3" t="n">
-        <v>111362</v>
-      </c>
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">287
-</t>
+          <t>Max.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">900
-</t>
+          <t>Min.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve">8243
-</t>
+          <t>(M+m)/2</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">87
-</t>
+          <t>Ampl.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1182
-</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
+          <t>Min. gazon</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Abri.</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t xml:space="preserve">29
-</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
+          <t>Ext.</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
-          <t xml:space="preserve">202
-</t>
+          <t>T</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t xml:space="preserve">201
-</t>
+          <t>T'a</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t xml:space="preserve">834
-</t>
+          <t>e.</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t xml:space="preserve">990
-</t>
+          <t>U</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t xml:space="preserve">02
-</t>
+          <t>∆e</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t xml:space="preserve">287
-</t>
+          <t>T</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t xml:space="preserve">241
-</t>
+          <t>T'a</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t xml:space="preserve">8
-</t>
+          <t>e.</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1689
-</t>
+          <t>U</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t xml:space="preserve">1122
-</t>
+          <t>∆e</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t xml:space="preserve">252
-</t>
+          <t>T</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t xml:space="preserve">228
-</t>
+          <t>T'a</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t xml:space="preserve">262
-</t>
+          <t>e.</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t xml:space="preserve">818
-</t>
+          <t>U</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t xml:space="preserve">8
-</t>
-        </is>
-      </c>
-      <c r="AA3" t="n">
-        <v>1</v>
-      </c>
+          <t>∆e</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="n">
+        <v>825</v>
+      </c>
       <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>12035</v>
-      </c>
+        <v>111362</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1396
+          <t xml:space="preserve">287
 </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">182
+          <t xml:space="preserve">900
 </t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve">254
+          <t xml:space="preserve">8243
 </t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">144
-</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">35
-</t>
-        </is>
-      </c>
+          <t xml:space="preserve">87
+</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1182
+</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1155
+          <t xml:space="preserve">29
 </t>
         </is>
       </c>
@@ -779,97 +793,98 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t xml:space="preserve">189
+          <t xml:space="preserve">202
 </t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t xml:space="preserve">188
+          <t xml:space="preserve">201
 </t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t xml:space="preserve">216
+          <t xml:space="preserve">834
 </t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t xml:space="preserve">0990
+          <t xml:space="preserve">990
 </t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t xml:space="preserve">09
+          <t xml:space="preserve">02
 </t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t xml:space="preserve">326
+          <t xml:space="preserve">287
 </t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t xml:space="preserve">254
+          <t xml:space="preserve">241
 </t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t xml:space="preserve">278
+          <t xml:space="preserve">8
 </t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1566
+          <t xml:space="preserve">1689
 </t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t xml:space="preserve">212
+          <t xml:space="preserve">1122
 </t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t xml:space="preserve">272
+          <t xml:space="preserve">252
 </t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t xml:space="preserve">240
+          <t xml:space="preserve">228
 </t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1278
+          <t xml:space="preserve">262
 </t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t xml:space="preserve">770
+          <t xml:space="preserve">818
 </t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t xml:space="preserve">82
+          <t xml:space="preserve">8
 </t>
         </is>
       </c>
       <c r="AA4" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AB4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -1010,6 +1025,9 @@
       <c r="AA5" t="n">
         <v>38</v>
       </c>
+      <c r="AB5" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -1155,6 +1173,9 @@
       <c r="AA6" t="n">
         <v>4</v>
       </c>
+      <c r="AB6" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1300,6 +1321,9 @@
       <c r="AA7" t="n">
         <v>5</v>
       </c>
+      <c r="AB7" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1446,6 +1470,9 @@
       </c>
       <c r="AA8" t="n">
         <v>109</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -1592,6 +1619,9 @@
       <c r="AA9" t="n">
         <v>101</v>
       </c>
+      <c r="AB9" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1741,6 +1771,9 @@
       <c r="AA10" t="n">
         <v>109</v>
       </c>
+      <c r="AB10" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1889,6 +1922,9 @@
       </c>
       <c r="AA11" t="n">
         <v>2</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -2032,6 +2068,9 @@
       <c r="AA12" t="n">
         <v>8</v>
       </c>
+      <c r="AB12" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -2181,6 +2220,9 @@
       <c r="AA13" t="n">
         <v>9</v>
       </c>
+      <c r="AB13" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -2328,6 +2370,9 @@
       <c r="AA14" t="n">
         <v>10</v>
       </c>
+      <c r="AB14" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2475,6 +2520,9 @@
       <c r="AA15" t="n">
         <v>701</v>
       </c>
+      <c r="AB15" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2610,6 +2658,9 @@
       <c r="AA16" t="n">
         <v>1107</v>
       </c>
+      <c r="AB16" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2759,6 +2810,9 @@
       <c r="AA17" t="n">
         <v>14</v>
       </c>
+      <c r="AB17" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2899,6 +2953,9 @@
       </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -3039,6 +3096,9 @@
         </is>
       </c>
       <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -3181,6 +3241,9 @@
       <c r="AA20" t="n">
         <v>149</v>
       </c>
+      <c r="AB20" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -3316,6 +3379,9 @@
       <c r="AA21" t="n">
         <v>15</v>
       </c>
+      <c r="AB21" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -3442,6 +3508,9 @@
       </c>
       <c r="AA22" t="n">
         <v>701</v>
+      </c>
+      <c r="AB22" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="23">
@@ -3587,6 +3656,9 @@
       </c>
       <c r="AA23" t="n">
         <v>108</v>
+      </c>
+      <c r="AB23" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -3700,6 +3772,9 @@
       <c r="AA24" t="n">
         <v>16</v>
       </c>
+      <c r="AB24" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -3837,6 +3912,9 @@
       <c r="AA25" t="n">
         <v>11</v>
       </c>
+      <c r="AB25" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -3979,6 +4057,9 @@
       <c r="AA26" t="n">
         <v>18</v>
       </c>
+      <c r="AB26" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -4126,6 +4207,9 @@
       <c r="AA27" t="n">
         <v>19</v>
       </c>
+      <c r="AB27" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
@@ -4268,6 +4352,9 @@
       <c r="AA28" t="n">
         <v>20</v>
       </c>
+      <c r="AB28" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -4416,6 +4503,9 @@
       </c>
       <c r="AA29" t="n">
         <v>101</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="30">
@@ -4547,6 +4637,9 @@
       <c r="AA30" t="n">
         <v>1514104</v>
       </c>
+      <c r="AB30" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
@@ -4692,6 +4785,9 @@
       <c r="AA31" t="n">
         <v>21</v>
       </c>
+      <c r="AB31" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -4835,6 +4931,9 @@
       </c>
       <c r="AA32" t="n">
         <v>22</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="33">
@@ -4978,6 +5077,9 @@
       <c r="AA33" t="n">
         <v>23</v>
       </c>
+      <c r="AB33" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -5120,6 +5222,9 @@
       <c r="AA34" t="n">
         <v>24</v>
       </c>
+      <c r="AB34" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -5260,6 +5365,9 @@
       </c>
       <c r="Z35" t="inlineStr"/>
       <c r="AA35" t="inlineStr"/>
+      <c r="AB35" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
@@ -5402,6 +5510,9 @@
       <c r="AA36" t="n">
         <v>101</v>
       </c>
+      <c r="AB36" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
@@ -5544,6 +5655,9 @@
       <c r="AA37" t="n">
         <v>28</v>
       </c>
+      <c r="AB37" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
@@ -5691,6 +5805,9 @@
       <c r="AA38" t="n">
         <v>26</v>
       </c>
+      <c r="AB38" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr"/>
@@ -5838,6 +5955,9 @@
       <c r="AA39" t="n">
         <v>28</v>
       </c>
+      <c r="AB39" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
@@ -5963,6 +6083,9 @@
       <c r="AA40" t="n">
         <v>5</v>
       </c>
+      <c r="AB40" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr"/>
@@ -6108,6 +6231,9 @@
       <c r="AA41" t="n">
         <v>30</v>
       </c>
+      <c r="AB41" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
@@ -6255,6 +6381,9 @@
       <c r="AA42" t="n">
         <v>31</v>
       </c>
+      <c r="AB42" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -6375,6 +6504,9 @@
       <c r="AA43" t="n">
         <v>1018</v>
       </c>
+      <c r="AB43" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
@@ -6519,6 +6651,9 @@
       </c>
       <c r="AA44" t="n">
         <v>1107</v>
+      </c>
+      <c r="AB44" t="n">
+        <v>43</v>
       </c>
     </row>
     <row r="45">
@@ -6611,6 +6746,9 @@
         </is>
       </c>
       <c r="AA45" t="inlineStr"/>
+      <c r="AB45" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
@@ -6748,6 +6886,9 @@
       <c r="AA46" t="n">
         <v>1108</v>
       </c>
+      <c r="AB46" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
@@ -6878,6 +7019,9 @@
       <c r="Y47" t="inlineStr"/>
       <c r="Z47" t="inlineStr"/>
       <c r="AA47" t="inlineStr"/>
+      <c r="AB47" t="n">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>